<commit_message>
Ajuste manejo de alertas
</commit_message>
<xml_diff>
--- a/usuarios.xlsx
+++ b/usuarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wgranados\Documents\Automatizacion\OTROS\linktic_technical_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BDA938-3C70-4C88-B169-F0B9BB4A83D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F9A6188-3CAA-4927-BC11-E99811C9B496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4AE48A74-ACAA-44AA-A803-31772F51D55E}"/>
   </bookViews>
@@ -47,23 +47,15 @@
     <t>Colombia123</t>
   </si>
   <si>
-    <t>Willian00008</t>
+    <t>Willian00020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -93,7 +85,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>